<commit_message>
Carry out visualization using WordCloud
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gioia\news_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroco\media_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E1994E-BEE5-4954-80F0-CE623E23F94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FB822E-725B-4952-A412-0FF8647B72DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{7A01D398-9565-48BC-9D55-440E7A73035D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{7A01D398-9565-48BC-9D55-440E7A73035D}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_corea" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1214" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="965">
   <si>
     <t>기사 제목</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5626,6 +5626,17 @@
   </si>
   <si>
     <t>https://www.repubblica.it/spettacoli/cinema/2021/04/20/news/marvel_trailer_shang-chi_e_la_leggenda_dei_dieci_anelli-297139400/?ref=search</t>
+  </si>
+  <si>
+    <t>Il 2022 è l’Anno della Tigre, secondo il calendario cinese. Un animale dalle caratteristiche positive, simbolo di forza e vitalità, coraggio ed eroismo. In zona Sarpi, la nostra Chinatown, le lanterne di carta accese ricordano che si celebra il Capodanno. Senza parata, sospesa per prudenza sanitaria, e senza particolari menu nei locali della zona. Ma la Tigre spinge a onorare la tradizione di festa in altri ristoranti cinesi, come il Giardino di Giada a un passo dal Duomo, da oltre 40 anni riferimento per l’autentica cucina del gigante asiatico e tra i preferiti dai cinesi che vengono a Milano, per lavoro o turismo. Gigi Chin segue la strada aperta da sua mamma Carmen. In tavola, piatti dello chef Zhao: involtini con ripieno di zucca, gnocchi di riso piccanti con polpa di granchio, gamberoni e branzino, galletto croccante.
+I noodles all’astice
+Nel menu di Capodanno del Bon Wei entra invece l’Amarone della Valpolicella. Sono state le Famiglie Storiche del celebre vitigno (riuniscono dieci cantine) a osare, in omaggio alla Tigre che suggerisce di uscire dagli schemi, l’inedito abbinamento con la cucina cinese. La complessità aromatica dell’Amarone — note di pepe, prugne secche, funghi e cacao — ben si sposa a piatti come la cernia gialla croccante, aglio nero, mandorle e peperoncino. O con l’anatra Yan Shui, preparata secondo lo stile di Nanchino, e i dessert di Sonia Latorre Ruiz. Mu Dim Sum accorda ogni piatto a un augurio di felicità e prosperità. Tradizione del locale, mai gradita come adesso. Così i noodles all’astice significano «la buona fortuna si avvicina», il messaggio della millefoglie, crema alla vaniglia, yuzu e gelato al sesamo è «spero che la tua casa sia piena d’oro e d’argento».
+Per festeggiare in intimità, c’è il piccolo locale Il Gusto della Nebbia. Punta sulla cucina tipica di Chongqing, città-regione con oltre 30 milioni di abitanti, nella Cina centro-meridionale. Da ordinare i noodles con germogli di bambù e zenzero saltati, senza brodo, o il riso con ragù di manzo allo Yuxiang accompagnati dal liquore di prugna verde. Gorillas, app di ultima generazione per la consegna della spesa in pochi minuti, festeggia l’Anno della Tigre con prodotti orientali, per far scoprire i sapori cinesi a casa. Chi li acquista avrà la guida scritta da Momoka Banana, influencer di origini cinesi che vive a Roma e si descrive «gialla fuori, bianca dentro». Giulia Liu e il team del Gong hanno creato un menu speciale. Comprende la «dim sum composta», mix di cinque piccoli ravioli al vapore, farciti con king crab, salmone, black cod, calamaro e curry; maiale caramellato nella soia dolce e i lamien (spaghetti), simbolo di longevità perché lunghi e tirati a mano, arricchiti con sugo all’astice. «E non manca il pesce», dice Giulia Liu, «presentato in un mosaico di crudo pregiato, filetti di tonno Balfegò, salmone selvaggio e ombrina. È ispirato a Mondrian, pensato come se l’artista fosse vissuto in Asia».</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>31 gennaio 2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -6109,8 +6120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F48C4D-9BF6-4D92-8B06-07B72B4C066C}">
   <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -10818,8 +10829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C190B168-A8E1-4057-A2ED-677FFCA3358F}">
   <dimension ref="A1:G169"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -11271,9 +11282,11 @@
       <c r="A24" s="2" t="s">
         <v>851</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>964</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>853</v>
+        <v>963</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>841</v>

</xml_diff>